<commit_message>
Change oil to Oil
</commit_message>
<xml_diff>
--- a/VT_EREG1_ELC_V12.xlsx
+++ b/VT_EREG1_ELC_V12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\DemoS_ADV_Stuttgart061118\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\ETSAP-Webinar\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A411AD6F-BA02-4892-AE37-E305CF0CB19F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E9CF43-574E-44C2-8F57-30EE0CA61DE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="570" windowWidth="25080" windowHeight="15030" tabRatio="901" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="901" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EB1" sheetId="133" r:id="rId1"/>
@@ -41,14 +41,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="O3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="2" shapeId="0">
+    <comment ref="P3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -261,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="2" shapeId="0">
+    <comment ref="Q3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -314,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="2" shapeId="0">
+    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -347,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P15" authorId="2" shapeId="0">
+    <comment ref="P15" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -440,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q15" authorId="1" shapeId="0">
+    <comment ref="Q15" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -465,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R15" authorId="2" shapeId="0">
+    <comment ref="R15" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -528,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="2" shapeId="0">
+    <comment ref="J16" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -776,14 +776,14 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="X3" authorId="0" shapeId="0">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -897,7 +897,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC3" authorId="1" shapeId="0">
+    <comment ref="AC3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -923,7 +923,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD3" authorId="2" shapeId="0">
+    <comment ref="AD3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -996,7 +996,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE3" authorId="2" shapeId="0">
+    <comment ref="AE3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1049,7 +1049,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF3" authorId="2" shapeId="0">
+    <comment ref="AF3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1082,7 +1082,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD9" authorId="2" shapeId="0">
+    <comment ref="AD9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1175,7 +1175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE9" authorId="1" shapeId="0">
+    <comment ref="AE9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1200,7 +1200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF9" authorId="2" shapeId="0">
+    <comment ref="AF9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1263,7 +1263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X10" authorId="2" shapeId="0">
+    <comment ref="X10" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1924,9 +1924,6 @@
     <t>Naphtha</t>
   </si>
   <si>
-    <t>Diesel oil</t>
-  </si>
-  <si>
     <t>~COMEMI</t>
   </si>
   <si>
@@ -2030,21 +2027,24 @@
   </si>
   <si>
     <t>~FI_T: Stock~2000</t>
+  </si>
+  <si>
+    <t>Diesel Oil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="186" formatCode="0.000"/>
-    <numFmt numFmtId="187" formatCode="General_)"/>
-    <numFmt numFmtId="188" formatCode="0.0"/>
-    <numFmt numFmtId="190" formatCode="0.0000"/>
-    <numFmt numFmtId="195" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="General_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2074,32 +2074,6 @@
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -2595,34 +2569,34 @@
   </borders>
   <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="123">
@@ -2644,18 +2618,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2664,11 +2638,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="9"/>
@@ -2682,69 +2656,69 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="29" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="29" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="22" fillId="9" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="22" fillId="9" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="20" fillId="7" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="9" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="18" fillId="9" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="16" fillId="7" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="7" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="7" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="7" borderId="18" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="7" borderId="18" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="7" borderId="19" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="7" borderId="19" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2753,23 +2727,23 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="188" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="4" fillId="16" borderId="0" xfId="16" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="14" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
@@ -2778,89 +2752,89 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="9" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="14" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="13" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="13" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="9" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="14" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="195" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="195" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="195" fontId="25" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="21" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="195" fontId="25" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="21" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="195" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="195" fontId="4" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2869,32 +2843,32 @@
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
-    <cellStyle name="Comma 2" xfId="5"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Input" xfId="7" builtinId="20"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="9"/>
-    <cellStyle name="Normal 2" xfId="10"/>
-    <cellStyle name="Normal 4" xfId="11"/>
-    <cellStyle name="Normal 4 2" xfId="12"/>
-    <cellStyle name="Normal 8" xfId="13"/>
-    <cellStyle name="Normal 9 2" xfId="14"/>
-    <cellStyle name="Normale_B2020" xfId="15"/>
+    <cellStyle name="Normal 10" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 4" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 4 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 8" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 9 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normale_B2020" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Percent" xfId="16" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="17"/>
-    <cellStyle name="Percent 3" xfId="18"/>
-    <cellStyle name="Percent 3 2" xfId="19"/>
-    <cellStyle name="Percent 3 3" xfId="20"/>
-    <cellStyle name="Percent 3 4" xfId="21"/>
-    <cellStyle name="Percent 4" xfId="22"/>
-    <cellStyle name="Percent 4 2" xfId="23"/>
-    <cellStyle name="Percent 4 3" xfId="24"/>
-    <cellStyle name="Percent 4 4" xfId="25"/>
-    <cellStyle name="Percent 5" xfId="26"/>
-    <cellStyle name="Percent 6" xfId="27"/>
-    <cellStyle name="Percent 7" xfId="28"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="29"/>
+    <cellStyle name="Percent 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Percent 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Percent 3 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Percent 3 3" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Percent 3 4" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Percent 4" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Percent 4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Percent 4 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Percent 4 4" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Percent 5" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Percent 6" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Percent 7" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4353,13 +4327,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4428,16 +4404,16 @@
         <v>45</v>
       </c>
       <c r="O2" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="P2" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q2" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="P2" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q2" s="48" t="s">
+      <c r="R2" s="48" t="s">
         <v>156</v>
-      </c>
-      <c r="R2" s="48" t="s">
-        <v>157</v>
       </c>
       <c r="S2" s="48" t="s">
         <v>46</v>
@@ -4449,11 +4425,11 @@
         <v>48</v>
       </c>
       <c r="V2" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X2" s="8"/>
       <c r="Y2" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z2" s="14" t="s">
         <v>68</v>
@@ -4476,7 +4452,7 @@
         <v>124</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>134</v>
@@ -4500,16 +4476,16 @@
         <v>51</v>
       </c>
       <c r="O3" s="49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P3" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q3" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="Q3" s="49" t="s">
+      <c r="R3" s="49" t="s">
         <v>153</v>
-      </c>
-      <c r="R3" s="49" t="s">
-        <v>154</v>
       </c>
       <c r="S3" s="49" t="s">
         <v>52</v>
@@ -5003,7 +4979,7 @@
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="C12" s="53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="53"/>
       <c r="E12" s="53"/>
@@ -5070,7 +5046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M5"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
@@ -5089,14 +5065,14 @@
     </row>
     <row r="2" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="4" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="E4" s="120" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F4" s="121"/>
       <c r="G4" s="121"/>
@@ -5109,7 +5085,7 @@
     </row>
     <row r="5" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E5" s="79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
@@ -5131,10 +5107,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5529,7 +5507,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="82" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15" s="80" t="s">
         <v>123</v>
@@ -5579,7 +5557,7 @@
         <v>33</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>34</v>
@@ -5588,7 +5566,7 @@
         <v>75</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J16" s="110" t="s">
         <v>36</v>
@@ -6042,13 +6020,13 @@
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="52"/>
       <c r="C32" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="68"/>
       <c r="C33" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -6060,10 +6038,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:AF65536"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -6195,7 +6173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:32" s="26" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:32" s="26" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="33" t="s">
         <v>107</v>
       </c>
@@ -6328,7 +6306,7 @@
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -6366,37 +6344,37 @@
         <v>6</v>
       </c>
       <c r="E9" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>164</v>
-      </c>
       <c r="G9" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="80" t="s">
         <v>167</v>
       </c>
-      <c r="H9" s="80" t="s">
+      <c r="I9" s="80" t="s">
         <v>168</v>
       </c>
-      <c r="I9" s="80" t="s">
+      <c r="J9" s="80" t="s">
         <v>169</v>
-      </c>
-      <c r="J9" s="80" t="s">
-        <v>170</v>
       </c>
       <c r="K9" s="80">
         <v>2030</v>
       </c>
       <c r="L9" s="80" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M9" s="80" t="s">
         <v>73</v>
       </c>
       <c r="N9" s="80" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O9" s="80" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P9" s="80" t="s">
         <v>72</v>
@@ -6408,7 +6386,7 @@
         <v>70</v>
       </c>
       <c r="S9" s="80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T9" s="80" t="s">
         <v>118</v>
@@ -6457,10 +6435,10 @@
         <v>33</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -6477,7 +6455,7 @@
         <v>82</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P10" s="19" t="s">
         <v>81</v>
@@ -6486,7 +6464,7 @@
         <v>105</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S10" s="19" t="s">
         <v>106</v>
@@ -7266,14 +7244,14 @@
     <row r="23" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B23" s="52"/>
       <c r="C23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V23" s="97"/>
     </row>
     <row r="24" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B24" s="68"/>
       <c r="C24" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V24" s="97"/>
     </row>
@@ -7333,7 +7311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7345,7 +7323,7 @@
   <sheetData>
     <row r="3" spans="2:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
@@ -7366,7 +7344,7 @@
     </row>
     <row r="5" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="41"/>
       <c r="F5" s="31"/>
@@ -7397,13 +7375,13 @@
         <v>76</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" s="88"/>
       <c r="G7" s="88"/>
@@ -7438,13 +7416,13 @@
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="52"/>
       <c r="C23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="68"/>
       <c r="C24" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>